<commit_message>
add AT-400 to aircraft data
</commit_message>
<xml_diff>
--- a/resources/AgAircraftData.xlsx
+++ b/resources/AgAircraftData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gill14/OneDrive - University of Illinois - Urbana/AccuProjects/Python Projects/AccuPatt/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gill14/Library/Mobile Documents/com~apple~CloudDocs/Projects/AccuPatt/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4738D552-2D11-C147-B92B-29BD4D30AEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F4AEF1-BDCF-4646-BEFA-BD8D26F11BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38160" yWindow="16520" windowWidth="21600" windowHeight="9740" tabRatio="792" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38160" yWindow="16520" windowWidth="21600" windowHeight="9740" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Air Tractor" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
   <si>
     <t>Model</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>188 AgPickup</t>
+  </si>
+  <si>
+    <t>AT-400</t>
   </si>
 </sst>
 </file>
@@ -601,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,29 +664,27 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B3">
         <v>400</v>
       </c>
       <c r="C3">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D9" si="0">C3*0.7</f>
-        <v>35.699999999999996</v>
+        <v>31.5</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E9" si="1">C3*0.25</f>
-        <v>12.75</v>
+        <v>11.25</v>
       </c>
       <c r="F3">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>400</v>
@@ -692,42 +693,42 @@
         <v>51</v>
       </c>
       <c r="D4">
+        <f t="shared" ref="D4:D10" si="0">C4*0.7</f>
+        <v>35.699999999999996</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E10" si="1">C4*0.25</f>
+        <v>12.75</v>
+      </c>
+      <c r="F4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5">
+        <v>400</v>
+      </c>
+      <c r="C5">
+        <v>51</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>35.699999999999996</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <f t="shared" si="1"/>
         <v>12.75</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>500</v>
-      </c>
-      <c r="C5">
-        <v>52</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>36.4</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>500</v>
@@ -743,13 +744,16 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
+      <c r="F6">
+        <v>140</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B7">
-        <v>485</v>
+        <v>500</v>
       </c>
       <c r="C7">
         <v>52</v>
@@ -765,45 +769,64 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B8">
-        <v>630</v>
+        <v>485</v>
       </c>
       <c r="C8">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>39.199999999999996</v>
+        <v>36.4</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>14</v>
-      </c>
-      <c r="F8">
-        <v>150</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9">
-        <v>800</v>
+        <v>630</v>
       </c>
       <c r="C9">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>41.3</v>
+        <v>39.199999999999996</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="F9">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>800</v>
+      </c>
+      <c r="C10">
+        <v>59</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>41.3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
         <v>14.75</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>160</v>
       </c>
     </row>
@@ -891,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -1478,11 +1501,11 @@
         <v>39</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D4" si="0">C2*0.7</f>
+        <f t="shared" ref="D2" si="0">C2*0.7</f>
         <v>27.299999999999997</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E4" si="1">C2*0.25</f>
+        <f t="shared" ref="E2" si="1">C2*0.25</f>
         <v>9.75</v>
       </c>
     </row>
@@ -1627,11 +1650,11 @@
         <v>35</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D3" si="0">C2*0.7</f>
+        <f t="shared" ref="D2" si="0">C2*0.7</f>
         <v>24.5</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E3" si="1">C2*0.25</f>
+        <f t="shared" ref="E2" si="1">C2*0.25</f>
         <v>8.75</v>
       </c>
     </row>
@@ -1689,11 +1712,11 @@
         <v>26</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D3" si="0">C2*0.7</f>
+        <f t="shared" ref="D2" si="0">C2*0.7</f>
         <v>18.2</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E3" si="1">C2*0.25</f>
+        <f t="shared" ref="E2" si="1">C2*0.25</f>
         <v>6.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add Thrush 510P2, 510P2+
</commit_message>
<xml_diff>
--- a/resources/AgAircraftData.xlsx
+++ b/resources/AgAircraftData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gill14/Library/Mobile Documents/com~apple~CloudDocs/Projects/AccuPatt/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F4AEF1-BDCF-4646-BEFA-BD8D26F11BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843180F3-4F9B-8A46-B279-72CBF556ACFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38160" yWindow="16520" windowWidth="21600" windowHeight="9740" tabRatio="792" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39640" yWindow="13700" windowWidth="21600" windowHeight="9740" tabRatio="792" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Air Tractor" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
   <si>
     <t>Model</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>AT-400</t>
+  </si>
+  <si>
+    <t>510P2</t>
+  </si>
+  <si>
+    <t>510P2+</t>
   </si>
 </sst>
 </file>
@@ -606,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
@@ -912,10 +918,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -959,11 +965,11 @@
         <v>44</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D8" si="0">C2*0.7</f>
+        <f t="shared" ref="D2:D10" si="0">C2*0.7</f>
         <v>30.799999999999997</v>
       </c>
       <c r="E2">
-        <f t="shared" ref="E2:E8" si="1">C2*0.25</f>
+        <f t="shared" ref="E2:E10" si="1">C2*0.25</f>
         <v>11</v>
       </c>
       <c r="F2">
@@ -994,7 +1000,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>510</v>
@@ -1003,11 +1009,11 @@
         <v>48</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D4:D5" si="2">C4*0.7</f>
         <v>33.599999999999994</v>
       </c>
       <c r="E4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="E4:E5" si="3">C4*0.25</f>
         <v>12</v>
       </c>
       <c r="F4">
@@ -1016,7 +1022,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="B5">
         <v>510</v>
@@ -1025,11 +1031,11 @@
         <v>48</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>33.599999999999994</v>
       </c>
       <c r="E5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="F5">
@@ -1038,10 +1044,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6">
-        <v>550</v>
+        <v>510</v>
       </c>
       <c r="C6">
         <v>48</v>
@@ -1060,42 +1066,86 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7">
-        <v>660</v>
+        <v>510</v>
       </c>
       <c r="C7">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D7">
-        <f>C7*0.7</f>
-        <v>37.799999999999997</v>
+        <f t="shared" si="0"/>
+        <v>33.599999999999994</v>
       </c>
       <c r="E7">
-        <f>C7*0.25</f>
-        <v>13.5</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B8">
-        <v>710</v>
+        <v>550</v>
       </c>
       <c r="C8">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>37.799999999999997</v>
+        <v>33.599999999999994</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>660</v>
+      </c>
+      <c r="C9">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <f>C9*0.7</f>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E9">
+        <f>C9*0.25</f>
         <v>13.5</v>
       </c>
-      <c r="F8">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10">
+        <v>710</v>
+      </c>
+      <c r="C10">
+        <v>54</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>13.5</v>
+      </c>
+      <c r="F10">
         <v>150</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Various Embraer Models to Pre-Loaded Aircraft
</commit_message>
<xml_diff>
--- a/resources/AgAircraftData.xlsx
+++ b/resources/AgAircraftData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10114"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gill14/Library/Mobile Documents/com~apple~CloudDocs/Projects/AccuPatt/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattgill/Library/Mobile Documents/com~apple~CloudDocs/iCloud/Projects/AccuPatt/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843180F3-4F9B-8A46-B279-72CBF556ACFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BE1A37-DC78-AA43-A8A6-1BF2E384CEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39640" yWindow="13700" windowWidth="21600" windowHeight="9740" tabRatio="792" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39640" yWindow="13700" windowWidth="21600" windowHeight="9740" tabRatio="792" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Air Tractor" sheetId="2" r:id="rId1"/>
@@ -20,11 +20,12 @@
     <sheet name="Grumman" sheetId="5" r:id="rId5"/>
     <sheet name="Hiller" sheetId="12" r:id="rId6"/>
     <sheet name="Hughes" sheetId="13" r:id="rId7"/>
-    <sheet name="Piper" sheetId="6" r:id="rId8"/>
-    <sheet name="PZL-Mielec" sheetId="7" r:id="rId9"/>
-    <sheet name="Robinson" sheetId="8" r:id="rId10"/>
-    <sheet name="Thrush" sheetId="9" r:id="rId11"/>
-    <sheet name="Weatherly" sheetId="10" r:id="rId12"/>
+    <sheet name="Ipanema" sheetId="14" r:id="rId8"/>
+    <sheet name="Piper" sheetId="6" r:id="rId9"/>
+    <sheet name="PZL-Mielec" sheetId="7" r:id="rId10"/>
+    <sheet name="Robinson" sheetId="8" r:id="rId11"/>
+    <sheet name="Thrush" sheetId="9" r:id="rId12"/>
+    <sheet name="Weatherly" sheetId="10" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="47">
   <si>
     <t>Model</t>
   </si>
@@ -180,6 +181,12 @@
   </si>
   <si>
     <t>510P2+</t>
+  </si>
+  <si>
+    <t>201A</t>
+  </si>
+  <si>
+    <t>202A</t>
   </si>
 </sst>
 </file>
@@ -842,6 +849,71 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>660</v>
+      </c>
+      <c r="C2">
+        <v>58</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2" si="0">C2*0.7</f>
+        <v>40.599999999999994</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2" si="1">C2*0.25</f>
+        <v>14.5</v>
+      </c>
+      <c r="F2">
+        <v>143</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -916,11 +988,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -1154,7 +1226,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -1569,7 +1641,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1776,6 +1848,104 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB2CCB33-45CE-644F-8257-EB603012DEE2}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>201</v>
+      </c>
+      <c r="B2">
+        <v>180</v>
+      </c>
+      <c r="C2">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3">
+        <v>180</v>
+      </c>
+      <c r="C3">
+        <v>36.299999999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>202</v>
+      </c>
+      <c r="B4">
+        <v>250</v>
+      </c>
+      <c r="C4">
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5">
+        <v>250</v>
+      </c>
+      <c r="C5">
+        <v>38.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>203</v>
+      </c>
+      <c r="B6">
+        <v>277</v>
+      </c>
+      <c r="C6">
+        <v>43.6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -1860,69 +2030,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>660</v>
-      </c>
-      <c r="C2">
-        <v>58</v>
-      </c>
-      <c r="D2">
-        <f t="shared" ref="D2" si="0">C2*0.7</f>
-        <v>40.599999999999994</v>
-      </c>
-      <c r="E2">
-        <f t="shared" ref="E2" si="1">C2*0.25</f>
-        <v>14.5</v>
-      </c>
-      <c r="F2">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>